<commit_message>
Trayectoria más corta en terminal
</commit_message>
<xml_diff>
--- a/src/data/Test.xlsx
+++ b/src/data/Test.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
   <si>
     <t>JuanPa</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>4, 1</t>
+  </si>
+  <si>
+    <t>Sutano</t>
   </si>
 </sst>
 </file>
@@ -88,7 +91,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -99,6 +102,9 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -388,6 +394,20 @@
       </c>
       <c r="E5" s="3"/>
     </row>
+    <row r="6">
+      <c r="A6" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="4">
+        <v>1.0</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>